<commit_message>
menambahkan preprocessing dataset part 1, membuat model cnn ke-2, dan merapikan direktory
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\semester 7\Pembelajaran Mesin\Tugas\Tugas Besar\ProjectML_261-235\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C156C75-3174-401B-90E8-35BEB18D9314}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCDE4BF-F3B9-42F9-81BF-DD2E0BF80DC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="62">
   <si>
     <t>Task</t>
   </si>
@@ -48,18 +48,6 @@
     <t>Ket Status</t>
   </si>
   <si>
-    <t>Dikerjakan</t>
-  </si>
-  <si>
-    <t>Selesai</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>Selesai dan Benar</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -126,9 +114,6 @@
     <t xml:space="preserve">Deployment </t>
   </si>
   <si>
-    <t>Error</t>
-  </si>
-  <si>
     <t>Tiara Intana Sari</t>
   </si>
   <si>
@@ -138,24 +123,12 @@
     <t>Colaborasi</t>
   </si>
   <si>
-    <t>Preprocessing Dataset 1</t>
-  </si>
-  <si>
-    <t>Modelling menggunakan Algoritma CNN 1</t>
-  </si>
-  <si>
     <t>Evaluasi Model CNN 2</t>
   </si>
   <si>
     <t>Evaluasi Model CNN 1</t>
   </si>
   <si>
-    <t>Modelling menggunakan Algoritma CNN 2</t>
-  </si>
-  <si>
-    <t>Preprocessing Dataset 2</t>
-  </si>
-  <si>
     <t>Modelling CNN 3 dan evaluasi</t>
   </si>
   <si>
@@ -183,9 +156,6 @@
     <t>Modelling CNN 7 HP 3</t>
   </si>
   <si>
-    <t>Preprocessing Dataset 3</t>
-  </si>
-  <si>
     <t>Modelling CNN 8 HP 4</t>
   </si>
   <si>
@@ -211,15 +181,42 @@
   </si>
   <si>
     <t>23.</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>On Going</t>
+  </si>
+  <si>
+    <t>Waiting</t>
+  </si>
+  <si>
+    <t>23-10-2021</t>
+  </si>
+  <si>
+    <t>25-10-2021</t>
+  </si>
+  <si>
+    <t>Preprocessing Dataset Part 1</t>
+  </si>
+  <si>
+    <t>Preprocessing Dataset  Part 2</t>
+  </si>
+  <si>
+    <t>Preprocessing Dataset Part 3</t>
+  </si>
+  <si>
+    <t>Modelling menggunakan Algoritma CNN Part 2</t>
+  </si>
+  <si>
+    <t>Modelling menggunakan Algoritma CNN Part 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -243,7 +240,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,18 +256,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -308,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -316,10 +301,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,17 +584,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:J25"/>
+  <dimension ref="A2:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.453125" customWidth="1"/>
     <col min="2" max="2" width="57.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" customWidth="1"/>
+    <col min="3" max="3" width="17.36328125" customWidth="1"/>
     <col min="4" max="4" width="15.1796875" customWidth="1"/>
     <col min="5" max="5" width="17.7265625" customWidth="1"/>
     <col min="6" max="6" width="17.81640625" bestFit="1" customWidth="1"/>
@@ -619,7 +603,7 @@
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -645,363 +629,392 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="J3" s="4" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+        <v>57</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="F4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="J4" s="5" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="D5" s="7"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="J5" s="6" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="J6" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="F7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="J7" s="8" t="s">
-        <v>10</v>
+        <v>30</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="F8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
+        <v>58</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+        <v>34</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
+        <v>39</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
+        <v>59</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
+        <v>40</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
+        <v>41</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
+        <v>42</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
+        <v>43</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
+        <v>38</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
+        <v>44</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
+        <v>19</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
+        <v>15</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
+        <v>20</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
+        <v>23</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
+        <v>25</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
+        <v>28</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D27" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
menambahkan model CNN pertama, mengedit sprint_project
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\semester 7\Pembelajaran Mesin\Tugas\Tugas Besar\ProjectML_261-235\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SEMESTER 7\PEMBELAJARAN MESIN\ProjectML_261-235\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCDE4BF-F3B9-42F9-81BF-DD2E0BF80DC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426A467B-30CB-4F31-92E7-A747F6116727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
   <si>
     <t>Task</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>Modelling menggunakan Algoritma CNN Part 1</t>
+  </si>
+  <si>
+    <t>22-10-2021</t>
   </si>
 </sst>
 </file>
@@ -587,21 +590,21 @@
   <dimension ref="A2:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.453125" customWidth="1"/>
-    <col min="2" max="2" width="57.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.36328125" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" customWidth="1"/>
-    <col min="5" max="5" width="17.7265625" customWidth="1"/>
-    <col min="6" max="6" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.90625" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -627,16 +630,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="2"/>
+      <c r="C3" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="F3" s="2" t="s">
         <v>29</v>
       </c>
@@ -647,7 +656,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -673,15 +682,22 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="2"/>
+      <c r="C5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F5" s="2" t="s">
         <v>29</v>
       </c>
@@ -692,16 +708,22 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="2"/>
+      <c r="C6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F6" s="2" t="s">
         <v>29</v>
       </c>
@@ -709,7 +731,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -732,7 +754,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -755,7 +777,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -770,7 +792,7 @@
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>45</v>
       </c>
@@ -785,7 +807,7 @@
       </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>46</v>
       </c>
@@ -800,7 +822,7 @@
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -815,7 +837,7 @@
       </c>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -830,7 +852,7 @@
       </c>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -845,7 +867,7 @@
       </c>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -860,7 +882,7 @@
       </c>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
@@ -875,7 +897,7 @@
       </c>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
@@ -890,7 +912,7 @@
       </c>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
@@ -905,7 +927,7 @@
       </c>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -920,7 +942,7 @@
       </c>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
@@ -935,7 +957,7 @@
       </c>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>37</v>
       </c>
@@ -950,7 +972,7 @@
       </c>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>48</v>
       </c>
@@ -965,7 +987,7 @@
       </c>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>49</v>
       </c>
@@ -980,7 +1002,7 @@
       </c>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>50</v>
       </c>
@@ -995,7 +1017,7 @@
       </c>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>51</v>
       </c>
@@ -1010,10 +1032,10 @@
       </c>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D26" s="9"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D27" s="9"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
menambahkan model VGG16 dengan menggunakan teknik preprocessing dataset berupa oversampling
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SEMESTER 7\PEMBELAJARAN MESIN\ProjectML_261-235\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\semester 7\Pembelajaran Mesin\Tugas\Tugas Besar\ProjectML_261-235\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426A467B-30CB-4F31-92E7-A747F6116727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3495B1-51D4-4638-9CB8-3F92182B65CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="66">
   <si>
     <t>Task</t>
   </si>
@@ -129,9 +129,6 @@
     <t>Evaluasi Model CNN 1</t>
   </si>
   <si>
-    <t>Modelling CNN 3 dan evaluasi</t>
-  </si>
-  <si>
     <t>17.</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>Preprocessing 4 (oversampling/undersampling)</t>
   </si>
   <si>
-    <t>Modelling CNN 4 dan evaluasi</t>
-  </si>
-  <si>
     <t>Modelling CNN  5 HP 1</t>
   </si>
   <si>
@@ -201,9 +195,6 @@
     <t>Preprocessing Dataset Part 1</t>
   </si>
   <si>
-    <t>Preprocessing Dataset  Part 2</t>
-  </si>
-  <si>
     <t>Preprocessing Dataset Part 3</t>
   </si>
   <si>
@@ -214,6 +205,24 @@
   </si>
   <si>
     <t>22-10-2021</t>
+  </si>
+  <si>
+    <t>Preprocessing Dataset  Part 2 (Balancing Class)</t>
+  </si>
+  <si>
+    <t>Modelling VGG16 dengan Oversampling Data</t>
+  </si>
+  <si>
+    <t>Modelling CNN dengan Oversampling Data</t>
+  </si>
+  <si>
+    <t>08-11-2021</t>
+  </si>
+  <si>
+    <t>09-11-2021</t>
+  </si>
+  <si>
+    <t>07-11-2021</t>
   </si>
 </sst>
 </file>
@@ -590,21 +599,21 @@
   <dimension ref="A2:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="57.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.453125" customWidth="1"/>
+    <col min="2" max="2" width="57.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" customWidth="1"/>
+    <col min="5" max="5" width="17.7265625" customWidth="1"/>
+    <col min="6" max="6" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -630,7 +639,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -638,77 +647,77 @@
         <v>9</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -716,45 +725,45 @@
         <v>33</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -762,87 +771,111 @@
         <v>32</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>65</v>
+      </c>
       <c r="F9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G9" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>64</v>
+      </c>
       <c r="F10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G10" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>64</v>
+      </c>
       <c r="F11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G11" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -852,12 +885,12 @@
       </c>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -867,12 +900,12 @@
       </c>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -882,12 +915,12 @@
       </c>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -897,12 +930,12 @@
       </c>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -912,12 +945,12 @@
       </c>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -927,9 +960,9 @@
       </c>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>19</v>
@@ -942,9 +975,9 @@
       </c>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>15</v>
@@ -957,9 +990,9 @@
       </c>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>20</v>
@@ -972,9 +1005,9 @@
       </c>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>23</v>
@@ -987,9 +1020,9 @@
       </c>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>25</v>
@@ -1002,9 +1035,9 @@
       </c>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>26</v>
@@ -1017,9 +1050,9 @@
       </c>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>28</v>
@@ -1032,10 +1065,10 @@
       </c>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D26" s="9"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D27" s="9"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add model using inceptionresnetv2 and update sprint project
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SEMESTER 7\PEMBELAJARAN MESIN\ProjectML_261-235\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23A6080-3F05-4424-AC68-82E03D912B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A949C0-F0DA-4E87-8455-5B4857F38E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
   <si>
     <t>Task</t>
   </si>
@@ -72,9 +72,6 @@
     <t>6.</t>
   </si>
   <si>
-    <t>Modelling menggunakan Algoritma Transfer Learning DenseNet169</t>
-  </si>
-  <si>
     <t xml:space="preserve">7. </t>
   </si>
   <si>
@@ -84,12 +81,6 @@
     <t>11.</t>
   </si>
   <si>
-    <t>Evaluasi Model Resnet50</t>
-  </si>
-  <si>
-    <t>Evaluasi Model DenseNet169</t>
-  </si>
-  <si>
     <t>12.</t>
   </si>
   <si>
@@ -138,9 +129,6 @@
     <t>19.</t>
   </si>
   <si>
-    <t>Preprocessing 4 (oversampling/undersampling)</t>
-  </si>
-  <si>
     <t>Model Resnet50</t>
   </si>
   <si>
@@ -220,6 +208,18 @@
   </si>
   <si>
     <t>Modelling CNN  dengan Hparams Tuning</t>
+  </si>
+  <si>
+    <t>18-12-2021</t>
+  </si>
+  <si>
+    <t>19-12-2021</t>
+  </si>
+  <si>
+    <t>Model VGG19 dengan Imporvisasi FC Layer</t>
+  </si>
+  <si>
+    <t>16-12-2021</t>
   </si>
 </sst>
 </file>
@@ -607,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,22 +656,22 @@
         <v>9</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -679,25 +679,25 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -705,25 +705,25 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -731,22 +731,22 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -754,22 +754,22 @@
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -777,306 +777,295 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="F15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>61</v>
+      </c>
       <c r="F16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G16" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G25" s="2"/>
     </row>

</xml_diff>